<commit_message>
took out fail plots
</commit_message>
<xml_diff>
--- a/check data.xlsx
+++ b/check data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sliang/git/om516-project-1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{91039F1C-6D77-9847-BF4C-06E6D759AAC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{969AFE3F-D632-9D4E-8CEC-49EC7EEDDA1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-34680" yWindow="-11740" windowWidth="34680" windowHeight="21100"/>
   </bookViews>
@@ -720,6 +720,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>xbar</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1302,6 +1327,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>range</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3357,8 +3407,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA1072"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G486" workbookViewId="0">
-      <selection activeCell="AE506" sqref="AE506"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="W477" sqref="W477"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>